<commit_message>
Add schedule to french page.
</commit_message>
<xml_diff>
--- a/en/schedule-beta/schedule.xlsx
+++ b/en/schedule-beta/schedule.xlsx
@@ -164,9 +164,6 @@
     </r>
   </si>
   <si>
-    <t>Keynote: Gil Bronza</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -787,6 +784,9 @@
 Room - Salle des Fêtes
 </t>
     </r>
+  </si>
+  <si>
+    <t>Keynote: Gil Broza</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1284,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1298,7 +1298,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1320,7 +1320,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -1337,7 +1337,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>4</v>
@@ -1348,7 +1348,7 @@
         <v>0.46875</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1359,16 +1359,16 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25" customHeight="1">
@@ -1376,7 +1376,7 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -1387,7 +1387,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -1398,7 +1398,7 @@
         <v>9.375E-2</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1409,16 +1409,16 @@
         <v>0.10416666666666667</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="25" customHeight="1">
@@ -1437,16 +1437,16 @@
         <v>0.17708333333333334</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" customHeight="1">
@@ -1454,7 +1454,7 @@
         <v>0.21875</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1465,7 +1465,7 @@
         <v>0.23958333333333334</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>

</xml_diff>